<commit_message>
making upload and download files and make excel import make
</commit_message>
<xml_diff>
--- a/public/download/product_bulk_demo.xlsx
+++ b/public/download/product_bulk_demo.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Super-Shop-Laravel\public\download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\php_seven_three\htdocs\rita-automobile\public\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA65D51-3B79-43EC-B402-966ECCDE29F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
@@ -75,16 +74,46 @@
     <t>current_stock</t>
   </si>
   <si>
-    <t>meta_title</t>
-  </si>
-  <si>
-    <t>meta_description</t>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>discount_type</t>
+  </si>
+  <si>
+    <t>part_no</t>
+  </si>
+  <si>
+    <t>segment_id</t>
+  </si>
+  <si>
+    <t>model_id</t>
+  </si>
+  <si>
+    <t>smart_part_no</t>
+  </si>
+  <si>
+    <t>ref_part_no</t>
+  </si>
+  <si>
+    <t>oe_part_no</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>mega_categories</t>
+  </si>
+  <si>
+    <t>series</t>
+  </si>
+  <si>
+    <t>percentage/amount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -403,11 +432,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,9 +453,10 @@
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
     <col min="11" max="11" width="23.7109375" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,8 +499,35 @@
       <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -503,6 +560,18 @@
       </c>
       <c r="L2">
         <v>10</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>